<commit_message>
Added more methods to Reader classes and refactored the code
</commit_message>
<xml_diff>
--- a/ExcelCSVReaderApp/TestData.xlsx
+++ b/ExcelCSVReaderApp/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\RiderProjects\ExcelCSVReaderApp\ExcelCSVReaderApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onimalarat\RiderProjects\CSharp_GemBox_Excel_CSV_Reader_App\ExcelCSVReaderApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B55C8C-FDD2-4624-A0F7-87FDC2DD7CEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B32B97-8FAB-4AB7-9915-096D1C9E8ED5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EBCD1ECD-8164-411B-9978-94E3A0535AF7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EBCD1ECD-8164-411B-9978-94E3A0535AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Key</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>Osanda</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A739083-8A35-4483-AAB7-7D9D8D7B29C4}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,9 +492,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9">
-        <v>1</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>